<commit_message>
push forgotten updates oopsies
</commit_message>
<xml_diff>
--- a/outputs/San Juan thermal mark application table.xlsx
+++ b/outputs/San Juan thermal mark application table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAVIDSONKA\Documents\ANALYSIS\Area20\A20\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{511CCFAC-5A55-41E9-8E0E-D04079F7EAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8336D0E-1D3E-419B-BAE2-B5F78D95C86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2865" yWindow="5640" windowWidth="21600" windowHeight="10905" xr2:uid="{E5D76997-CF60-48C2-AE4F-9AC555D85A1D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{E5D76997-CF60-48C2-AE4F-9AC555D85A1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -111,9 +111,6 @@
     <t>2yo BY</t>
   </si>
   <si>
-    <t>thermal unmarked BYs</t>
-  </si>
-  <si>
     <t>good quality thermal marked BYs</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>6yo BY</t>
+  </si>
+  <si>
+    <t>no thermal mark BYs</t>
   </si>
 </sst>
 </file>
@@ -511,15 +511,15 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -536,10 +536,10 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2012</v>
       </c>
@@ -564,7 +564,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2013</v>
       </c>
@@ -589,10 +589,10 @@
         <v>2007</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2014</v>
       </c>
@@ -617,10 +617,10 @@
         <v>2008</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2015</v>
       </c>
@@ -645,10 +645,10 @@
         <v>2009</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2016</v>
       </c>
@@ -673,7 +673,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2017</v>
       </c>
@@ -698,7 +698,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2018</v>
       </c>
@@ -723,7 +723,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2019</v>
       </c>
@@ -748,7 +748,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2020</v>
       </c>
@@ -773,7 +773,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2021</v>
       </c>
@@ -798,7 +798,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2022</v>
       </c>
@@ -823,7 +823,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2023</v>
       </c>

</xml_diff>